<commit_message>
vault backup: 2025-11-02 21:43:23
</commit_message>
<xml_diff>
--- a/02 Master/S1 TU Dresden/Horario.xlsx
+++ b/02 Master/S1 TU Dresden/Horario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan\Documents\Obsidian Vault\Apuntes\02 Master\S1 TU Dresden\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20BE1644-F297-4F1A-B717-B76636DA1A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5A6E71-0F35-4C63-98BA-267F78FFBFCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -109,7 +109,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -122,6 +122,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="24">
     <border>
@@ -448,7 +454,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -462,19 +468,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -483,40 +510,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -894,8 +903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10:H11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -928,7 +937,7 @@
       </c>
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="19" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="1"/>
@@ -937,140 +946,142 @@
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="6"/>
+      <c r="H4" s="5"/>
     </row>
     <row r="5" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="5"/>
-      <c r="D5" s="9"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="7"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="20"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="13"/>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="10" t="s">
+      <c r="E6" s="9"/>
+      <c r="F6" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="17" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="7"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="22"/>
-      <c r="H8" s="23" t="s">
+      <c r="G8" s="15"/>
+      <c r="H8" s="16" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="7"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="6"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="5"/>
     </row>
     <row r="10" spans="3:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="10" t="s">
+      <c r="G10" s="6"/>
+      <c r="H10" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="7"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="11"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="18"/>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="21"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="14"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="6"/>
+      <c r="H12" s="5"/>
     </row>
     <row r="13" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C13" s="7"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="8"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="6"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="6"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="5"/>
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="16" t="s">
+      <c r="E14" s="6"/>
+      <c r="F14" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="18"/>
+      <c r="H14" s="11"/>
     </row>
     <row r="15" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="12"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="19"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="H6:H7"/>
@@ -1087,8 +1098,6 @@
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="F6:F7"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="F10:F11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>